<commit_message>
Sex Ratio Descriptive Table
</commit_message>
<xml_diff>
--- a/sr_tables.xlsx
+++ b/sr_tables.xlsx
@@ -99,6 +99,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +151,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,7 +160,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,24 +441,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="3" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="4" t="s">
@@ -464,9 +466,8 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -485,11 +486,11 @@
       <c r="F2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -508,11 +509,11 @@
       <c r="F3" s="2">
         <v>0.87224590000000002</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0.1411473</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -531,11 +532,11 @@
       <c r="F4" s="2">
         <v>0.68282569999999998</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>0.31866303000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -554,11 +555,11 @@
       <c r="F5" s="2">
         <v>1.1195063000000001</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>-0.26767091999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -577,11 +578,11 @@
       <c r="F6" s="2">
         <v>0.46477619999999997</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>-6.4995399999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -600,11 +601,11 @@
       <c r="F7" s="2">
         <v>1.116827</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>0.62198072000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -623,11 +624,11 @@
       <c r="F8" s="2">
         <v>0.50672309999999998</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>0.73839071999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -646,11 +647,11 @@
       <c r="F9" s="2">
         <v>0.7125146</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>0.38693746000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -669,13 +670,13 @@
       <c r="F10" s="7">
         <v>0.27613399999999999</v>
       </c>
-      <c r="G10" s="7">
+      <c r="H10" s="7">
         <v>-0.73220686999999995</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
A few more SSR charts.
</commit_message>
<xml_diff>
--- a/sr_tables.xlsx
+++ b/sr_tables.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SSRs" sheetId="1" r:id="rId1"/>
+    <sheet name="Period SRX" sheetId="2" r:id="rId2"/>
+    <sheet name="Cohort SRX" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>Sweden</t>
   </si>
@@ -89,18 +91,79 @@
     <t>Std. Dev. * 100</t>
   </si>
   <si>
-    <t>Pearson's r with Year</t>
-  </si>
-  <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>1921-2014</t>
+  </si>
+  <si>
+    <t>1992-2005</t>
+  </si>
+  <si>
+    <t>1872-2014</t>
+  </si>
+  <si>
+    <t>1947-2014</t>
+  </si>
+  <si>
+    <t>Sex Ratio Crossovers</t>
+  </si>
+  <si>
+    <t>Std. Dev.</t>
+  </si>
+  <si>
+    <t>1850-1966</t>
+  </si>
+  <si>
+    <t>1921-1964</t>
+  </si>
+  <si>
+    <t>1872-1964</t>
+  </si>
+  <si>
+    <t>1947-1964</t>
+  </si>
+  <si>
+    <t>1959-1964</t>
+  </si>
+  <si>
+    <t>1933-1965</t>
+  </si>
+  <si>
+    <t>Years Without Cross</t>
+  </si>
+  <si>
+    <t>Cohorts Without Cross</t>
+  </si>
+  <si>
+    <t>1956-1963</t>
+  </si>
+  <si>
+    <t>1954-1963</t>
+  </si>
+  <si>
+    <t>1950-1965</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Available Cohorts</t>
+  </si>
+  <si>
+    <t>1873-1879, 1883-1893</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -148,19 +211,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,43 +518,39 @@
     <col min="3" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -509,11 +569,8 @@
       <c r="F3" s="2">
         <v>0.87224590000000002</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.1411473</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -532,11 +589,8 @@
       <c r="F4" s="2">
         <v>0.68282569999999998</v>
       </c>
-      <c r="H4" s="2">
-        <v>0.31866303000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -555,11 +609,8 @@
       <c r="F5" s="2">
         <v>1.1195063000000001</v>
       </c>
-      <c r="H5" s="2">
-        <v>-0.26767091999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -578,11 +629,8 @@
       <c r="F6" s="2">
         <v>0.46477619999999997</v>
       </c>
-      <c r="H6" s="2">
-        <v>-6.4995399999999998E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -601,11 +649,8 @@
       <c r="F7" s="2">
         <v>1.116827</v>
       </c>
-      <c r="H7" s="2">
-        <v>0.62198072000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -624,11 +669,8 @@
       <c r="F8" s="2">
         <v>0.50672309999999998</v>
       </c>
-      <c r="H8" s="2">
-        <v>0.73839071999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -647,31 +689,25 @@
       <c r="F9" s="2">
         <v>0.7125146</v>
       </c>
-      <c r="H9" s="2">
-        <v>0.38693746000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>1.0456859999999999</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>1.05854</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>1.050989</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>0.27613399999999999</v>
-      </c>
-      <c r="H10" s="7">
-        <v>-0.73220686999999995</v>
       </c>
     </row>
   </sheetData>
@@ -680,4 +716,466 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>98</v>
+      </c>
+      <c r="F3" s="6">
+        <v>51.934100000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <v>12.053057000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>67</v>
+      </c>
+      <c r="F4" s="6">
+        <v>55.117019999999997</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4.7266260000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
+      </c>
+      <c r="F5" s="6">
+        <v>48.5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>2.5038429999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>98</v>
+      </c>
+      <c r="F6" s="6">
+        <v>56.247999999999998</v>
+      </c>
+      <c r="G6" s="6">
+        <v>14.37777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>47</v>
+      </c>
+      <c r="E7">
+        <v>63</v>
+      </c>
+      <c r="F7" s="6">
+        <v>56.985289999999999</v>
+      </c>
+      <c r="G7" s="6">
+        <v>2.9749829999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6">
+        <v>33.142859999999999</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2.5185029999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>71</v>
+      </c>
+      <c r="F9" s="6">
+        <v>53.053890000000003</v>
+      </c>
+      <c r="G9" s="6">
+        <v>13.979873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>56</v>
+      </c>
+      <c r="F10" s="6">
+        <v>48.698799999999999</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3.180485</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3" s="6">
+        <v>47.723480000000002</v>
+      </c>
+      <c r="G3" s="6">
+        <v>11.6199014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <v>61</v>
+      </c>
+      <c r="F4" s="6">
+        <v>51.68571</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4.5682498999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>63</v>
+      </c>
+      <c r="F5" s="6">
+        <v>42.869050000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <v>14.009273800000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>58</v>
+      </c>
+      <c r="F6" s="6">
+        <v>56.142859999999999</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.069045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+      <c r="F7" s="6">
+        <v>32</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.63245549999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8" s="6">
+        <v>51.48</v>
+      </c>
+      <c r="G8" s="6">
+        <v>11.1423117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1965</v>
+      </c>
+      <c r="D9">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>51</v>
+      </c>
+      <c r="F9" s="6">
+        <v>45.5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>2.0790817000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>